<commit_message>
Upload Data, Affected Station Fixes, Media Release Widgets
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Cargo.xlsx
+++ b/src/assets/static-content/Cargo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Indigo ERS Source code\ERS\Release\Post-GoLive\CMS.Web\DownloadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PAL_CMS_Git_03052017\ERSClient\src\assets\static-content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Flight Details</t>
   </si>
@@ -35,13 +35,43 @@
     <t>POL</t>
   </si>
   <si>
-    <t>Manifest Pieces</t>
-  </si>
-  <si>
-    <t>Manifest Weight</t>
-  </si>
-  <si>
     <t>AWB</t>
+  </si>
+  <si>
+    <t>Manifest Pieces(Please Enter Numaric Value)</t>
+  </si>
+  <si>
+    <t>Manifest Weight(Please Enter Numaric Value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipper’s Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipper’s Address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipper’s Contact Number </t>
+  </si>
+  <si>
+    <t>Consignee's Name</t>
+  </si>
+  <si>
+    <t>Consignee's Address</t>
+  </si>
+  <si>
+    <t>Consignee's Contact Number</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Cargo Type</t>
+  </si>
+  <si>
+    <t>Advisory To Consignee</t>
   </si>
 </sst>
 </file>
@@ -375,18 +405,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -397,16 +438,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Media Release Optimization & Demand fix
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Cargo.xlsx
+++ b/src/assets/static-content/Cargo.xlsx
@@ -38,12 +38,6 @@
     <t>AWB</t>
   </si>
   <si>
-    <t>Manifest Pieces(Please Enter Numaric Value)</t>
-  </si>
-  <si>
-    <t>Manifest Weight(Please Enter Numaric Value)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shipper’s Name </t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>Advisory To Consignee</t>
+  </si>
+  <si>
+    <t>Manifest Pieces</t>
+  </si>
+  <si>
+    <t>Manifest Weight</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
     <col min="16" max="16" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -441,40 +441,40 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>